<commit_message>
More tokens & small fixes
</commit_message>
<xml_diff>
--- a/Tables.xlsx
+++ b/Tables.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="92">
   <si>
     <t>Token Name</t>
   </si>
@@ -300,6 +300,12 @@
   </si>
   <si>
     <t>: whitespace</t>
+  </si>
+  <si>
+    <t>Latex Rule</t>
+  </si>
+  <si>
+    <t>[a-zA-Z0-9]+ ":" ([0-9A-Z\_.]+ $\mid$ "'" ([0-9A-Z\_ !@\#\$\%\textasciicircum{}\&amp;*()\-+=\{\}:;$\mid$\textless\textgreater,./?\textbackslash{}\textbackslash{}] $\mid$ `''')+  `\ '\ ') `!'</t>
   </si>
 </sst>
 </file>
@@ -625,10 +631,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -639,7 +645,7 @@
     <col min="5" max="5" width="14.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -655,8 +661,11 @@
       <c r="E1" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>36</v>
       </c>
@@ -673,7 +682,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -690,7 +699,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -707,7 +716,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -724,7 +733,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>29</v>
       </c>
@@ -741,7 +750,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -759,7 +768,7 @@
       </c>
       <c r="F7" s="2"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -776,7 +785,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>27</v>
       </c>
@@ -793,8 +802,11 @@
         <v>65</v>
       </c>
       <c r="F9" s="2"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G9" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>23</v>
       </c>
@@ -811,7 +823,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="28.55" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="28.55" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>32</v>
       </c>
@@ -828,7 +840,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="28.55" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="28.55" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -845,7 +857,7 @@
         <v>10.1</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>77</v>
       </c>
@@ -862,7 +874,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -879,7 +891,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>30</v>
       </c>
@@ -896,7 +908,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>25</v>
       </c>

</xml_diff>

<commit_message>
First draft of chapter 2
</commit_message>
<xml_diff>
--- a/Tables.xlsx
+++ b/Tables.xlsx
@@ -126,9 +126,6 @@
     <t>"_xlnm." [A-Z_]+</t>
   </si>
   <si>
-    <t>NAMED_RANGE_PREFIXED</t>
-  </si>
-  <si>
     <t>("TRUE" | "FALSE" | [A-Z]+[0-9]+) [A-Z_][A-Za-z0-9_.]*</t>
   </si>
   <si>
@@ -306,6 +303,9 @@
   </si>
   <si>
     <t>[a-zA-Z0-9]+ ":" ([0-9A-Z\_.]+ $\mid$ "'" ([0-9A-Z\_ !@\#\$\%\textasciicircum{}\&amp;*()\-+=\{\}:;$\mid$\textless\textgreater,./?\textbackslash{}\textbackslash{}] $\mid$ `''')+  `\ '\ ') `!'</t>
+  </si>
+  <si>
+    <t>NAMED_RANGE_COMBINED</t>
   </si>
 </sst>
 </file>
@@ -634,7 +634,7 @@
   <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -643,6 +643,7 @@
     <col min="2" max="2" width="33.375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="73.375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="151.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -653,33 +654,33 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D1" t="s">
         <v>4</v>
       </c>
       <c r="E1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D2">
         <v>0</v>
       </c>
       <c r="E2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -687,7 +688,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C3" t="s">
         <v>8</v>
@@ -704,7 +705,7 @@
         <v>21</v>
       </c>
       <c r="B4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C4" t="s">
         <v>22</v>
@@ -713,7 +714,7 @@
         <v>2</v>
       </c>
       <c r="E4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -721,7 +722,7 @@
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C5" t="s">
         <v>7</v>
@@ -738,16 +739,16 @@
         <v>29</v>
       </c>
       <c r="B6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D6">
         <v>5</v>
       </c>
       <c r="E6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -755,7 +756,7 @@
         <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C7" t="s">
         <v>15</v>
@@ -764,7 +765,7 @@
         <v>5</v>
       </c>
       <c r="E7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F7" s="2"/>
     </row>
@@ -773,7 +774,7 @@
         <v>18</v>
       </c>
       <c r="B8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C8" t="s">
         <v>20</v>
@@ -782,7 +783,7 @@
         <v>0</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -790,7 +791,7 @@
         <v>27</v>
       </c>
       <c r="B9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C9" t="s">
         <v>28</v>
@@ -799,11 +800,11 @@
         <v>1</v>
       </c>
       <c r="E9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F9" s="2"/>
       <c r="G9" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -811,7 +812,7 @@
         <v>23</v>
       </c>
       <c r="B10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C10" t="s">
         <v>24</v>
@@ -820,24 +821,24 @@
         <v>-2</v>
       </c>
       <c r="E10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="28.55" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>91</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C11" t="s">
         <v>32</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C11" t="s">
-        <v>33</v>
       </c>
       <c r="D11">
         <v>3</v>
       </c>
       <c r="E11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="28.55" x14ac:dyDescent="0.25">
@@ -845,7 +846,7 @@
         <v>10</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C12" t="s">
         <v>5</v>
@@ -859,19 +860,19 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C13" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D13">
         <v>5</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -879,7 +880,7 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C14" t="s">
         <v>13</v>
@@ -888,7 +889,7 @@
         <v>5</v>
       </c>
       <c r="E14" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -896,7 +897,7 @@
         <v>30</v>
       </c>
       <c r="B15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C15" t="s">
         <v>31</v>
@@ -905,7 +906,7 @@
         <v>-1</v>
       </c>
       <c r="E15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -913,7 +914,7 @@
         <v>25</v>
       </c>
       <c r="B16" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C16" t="s">
         <v>26</v>
@@ -922,7 +923,7 @@
         <v>5</v>
       </c>
       <c r="E16" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -930,7 +931,7 @@
         <v>9</v>
       </c>
       <c r="B17" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C17" t="s">
         <v>11</v>
@@ -939,15 +940,15 @@
         <v>0</v>
       </c>
       <c r="E17" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B18" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C18" t="s">
         <v>2</v>
@@ -961,27 +962,27 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B19" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D19">
         <v>0</v>
       </c>
       <c r="E19" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B20" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C20" t="s">
         <v>17</v>
@@ -990,7 +991,7 @@
         <v>4</v>
       </c>
       <c r="E20" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -998,7 +999,7 @@
         <v>16</v>
       </c>
       <c r="B21" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C21" t="s">
         <v>19</v>
@@ -1007,7 +1008,7 @@
         <v>0</v>
       </c>
       <c r="E21" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -1038,15 +1039,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B1" t="s">
         <v>80</v>
-      </c>
-      <c r="B1" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -1054,7 +1055,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -1062,7 +1063,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -1070,7 +1071,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B5">
         <v>4</v>
@@ -1078,7 +1079,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B6">
         <v>5</v>
@@ -1094,7 +1095,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B8">
         <v>7</v>
@@ -1102,7 +1103,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B9">
         <v>8</v>

</xml_diff>